<commit_message>
update: modify data insied .xlsx file lecture 14, 17
</commit_message>
<xml_diff>
--- a/Week 13 Lecture.xlsx
+++ b/Week 13 Lecture.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\FoS-POE-2\FoS-POE2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E9591E-4680-4424-83D5-8C8291640E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="16275" windowHeight="7485"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formatting" sheetId="3" r:id="rId1"/>
@@ -16,20 +22,28 @@
   <definedNames>
     <definedName name="cement" localSheetId="0">Formatting!$B$7:$G$12</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Connection" type="4" refreshedVersion="1" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Connection" type="4" refreshedVersion="1" background="1" saveData="1">
     <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://www.stat.ncsu.edu/sas/sicl/data/cement.dat" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="165">
   <si>
     <t>Practice: Formulas</t>
   </si>
@@ -455,20 +469,90 @@
   </si>
   <si>
     <t>Are both Q1 and Q2 lower than Q3?</t>
+  </si>
+  <si>
+    <t>JAN</t>
+  </si>
+  <si>
+    <t>FEB</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>APR</t>
+  </si>
+  <si>
+    <t>MAY</t>
+  </si>
+  <si>
+    <t>JUN</t>
+  </si>
+  <si>
+    <t>JUL</t>
+  </si>
+  <si>
+    <t>AUG</t>
+  </si>
+  <si>
+    <t>SEP</t>
+  </si>
+  <si>
+    <t>OCT</t>
+  </si>
+  <si>
+    <t>NOV</t>
+  </si>
+  <si>
+    <t>DEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Fruit of the Loom Girl's Socks" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Rawlings Little League Baseball" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Secret Antiperspirant" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Deadpool DVD" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Maxwell House Coffee 28 oz" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Banana Boat Sunscreen,  8 oz" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Wrench Set, 18 pieces" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "M and M, 42 oz" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Bertoli Alfredo Sauce" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Large Paperclips, 10 boxes" </t>
+  </si>
+  <si>
+    <t> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="6">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -949,11 +1033,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1047,7 +1132,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1057,7 +1141,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1117,17 +1200,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1142,6 +1224,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1164,7 +1249,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Text Box 1"/>
+        <xdr:cNvPr id="2" name="Text Box 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1271,7 +1362,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1334,7 +1431,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Text Box 4"/>
+        <xdr:cNvPr id="4" name="Text Box 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1396,7 +1499,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 3"/>
+        <xdr:cNvPr id="5" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1459,7 +1568,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Text Box 1"/>
+        <xdr:cNvPr id="7" name="Text Box 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1536,7 +1651,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1579,7 +1700,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Text Box 1"/>
+        <xdr:cNvPr id="2" name="Text Box 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2012,7 +2139,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 4"/>
+        <xdr:cNvPr id="3" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2075,7 +2208,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Text Box 5"/>
+        <xdr:cNvPr id="4" name="Text Box 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2458,7 +2597,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 8"/>
+        <xdr:cNvPr id="5" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2513,7 +2658,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Text Box 9"/>
+        <xdr:cNvPr id="6" name="Text Box 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2738,7 +2889,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Text Box 10"/>
+        <xdr:cNvPr id="7" name="Text Box 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2963,7 +3120,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Text Box 12"/>
+        <xdr:cNvPr id="9" name="Text Box 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3394,7 +3557,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Text Box 13"/>
+        <xdr:cNvPr id="10" name="Text Box 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3659,7 +3828,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Text Box 10"/>
+        <xdr:cNvPr id="11" name="Text Box 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3725,7 +3900,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cement" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cement" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3771,7 +3946,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3804,9 +3979,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3839,6 +4031,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4014,20 +4223,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="18">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -4037,18 +4247,23 @@
       <c r="F2" s="48"/>
       <c r="G2" s="48"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="49" t="s">
+    <row r="6" spans="1:11">
+      <c r="B6" s="90" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="50">
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" s="49">
         <v>1</v>
       </c>
       <c r="C7" s="1">
@@ -4061,10 +4276,10 @@
         <v>11.8</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="51"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="52">
+      <c r="G7" s="50"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="B8" s="51">
         <v>2</v>
       </c>
       <c r="C8" s="2">
@@ -4077,10 +4292,10 @@
         <v>24.7</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="53"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="52">
+      <c r="G8" s="52"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="B9" s="51">
         <v>3</v>
       </c>
       <c r="C9" s="2">
@@ -4095,12 +4310,12 @@
       <c r="F9" s="2">
         <v>24.2</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="52">
         <v>26.2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="52">
+    <row r="10" spans="1:11">
+      <c r="B10" s="51">
         <v>7</v>
       </c>
       <c r="C10" s="2">
@@ -4115,15 +4330,15 @@
       <c r="F10" s="2">
         <v>33.1</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="52">
         <v>35.700000000000003</v>
       </c>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="55">
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="B11" s="54">
         <v>28</v>
       </c>
       <c r="C11" s="3">
@@ -4138,267 +4353,310 @@
       <c r="F11" s="3">
         <v>35.700000000000003</v>
       </c>
-      <c r="G11" s="56">
+      <c r="G11" s="55">
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="57" t="s">
+    <row r="13" spans="1:11">
+      <c r="B13" s="56" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18">
+    <row r="18" spans="1:10">
+      <c r="B18" s="91">
         <v>100</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19">
+    <row r="19" spans="1:10">
+      <c r="B19" s="91">
         <v>100</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="57" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20">
+    <row r="20" spans="1:10">
+      <c r="B20" s="91">
         <v>1000000</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="57" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="59">
+    <row r="21" spans="1:10">
+      <c r="B21" s="91">
         <v>100</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="57" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="59">
+    <row r="22" spans="1:10">
+      <c r="B22" s="91">
         <v>100</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="57" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="B29" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="62">
+      <c r="C29" s="60">
         <v>2010</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="60">
         <v>2011</v>
       </c>
-      <c r="E29" s="62">
+      <c r="E29" s="60">
         <v>2012</v>
       </c>
-      <c r="F29" s="62">
+      <c r="F29" s="60">
         <v>2013</v>
       </c>
-      <c r="G29" s="62">
+      <c r="G29" s="60">
         <v>2014</v>
       </c>
-      <c r="H29" s="62">
+      <c r="H29" s="60">
         <v>2015</v>
       </c>
-      <c r="I29" s="62">
+      <c r="I29" s="60">
         <v>2016</v>
       </c>
-      <c r="J29" s="62">
+      <c r="J29" s="60">
         <v>2017</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="B30" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="63">
+      <c r="C30" s="61">
         <v>9785</v>
       </c>
-      <c r="D30" s="63">
+      <c r="D30" s="61">
         <v>7672</v>
       </c>
-      <c r="E30" s="63">
+      <c r="E30" s="61">
         <v>9141</v>
       </c>
-      <c r="F30" s="63">
+      <c r="F30" s="61">
         <v>9507</v>
       </c>
-      <c r="G30" s="63">
+      <c r="G30" s="61">
         <v>5693</v>
       </c>
-      <c r="H30" s="63">
+      <c r="H30" s="61">
         <v>8380</v>
       </c>
-      <c r="I30" s="63">
+      <c r="I30" s="61">
         <v>8319</v>
       </c>
-      <c r="J30" s="63">
+      <c r="J30" s="61">
         <v>7908</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="62" t="s">
+    <row r="32" spans="1:10">
+      <c r="B32" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="62" t="s">
+      <c r="C32" s="60" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="61"/>
-      <c r="C38" s="61"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="61"/>
-      <c r="C39" s="61"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="61"/>
-      <c r="C40" s="61"/>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="60">
+        <v>2010</v>
+      </c>
+      <c r="C34" s="61">
+        <v>9785</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="60">
+        <v>2011</v>
+      </c>
+      <c r="C35" s="61">
+        <v>7672</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="60">
+        <v>2012</v>
+      </c>
+      <c r="C36" s="61">
+        <v>9141</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="60">
+        <v>2013</v>
+      </c>
+      <c r="C37" s="61">
+        <v>9507</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="60">
+        <v>2014</v>
+      </c>
+      <c r="C38" s="61">
+        <v>5693</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="60">
+        <v>2015</v>
+      </c>
+      <c r="C39" s="61">
+        <v>8380</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="60">
+        <v>2016</v>
+      </c>
+      <c r="C40" s="61">
+        <v>8319</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="60">
+        <v>2017</v>
+      </c>
+      <c r="C41" s="61">
+        <v>7908</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:G6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:M120"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="259" max="259" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="515" max="515" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="771" max="771" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="1027" max="1027" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="1283" max="1283" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="1539" max="1539" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="1795" max="1795" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2051" max="2051" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2307" max="2307" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2563" max="2563" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2819" max="2819" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3075" max="3075" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3331" max="3331" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3587" max="3587" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3843" max="3843" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4099" max="4099" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4355" max="4355" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4611" max="4611" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4867" max="4867" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5123" max="5123" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5379" max="5379" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5635" max="5635" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5891" max="5891" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6147" max="6147" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6403" max="6403" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6659" max="6659" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6915" max="6915" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7171" max="7171" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7427" max="7427" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7683" max="7683" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7939" max="7939" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8195" max="8195" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8451" max="8451" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8707" max="8707" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8963" max="8963" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9219" max="9219" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9475" max="9475" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9731" max="9731" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9987" max="9987" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10243" max="10243" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10499" max="10499" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10755" max="10755" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11011" max="11011" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11267" max="11267" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11523" max="11523" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11779" max="11779" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12035" max="12035" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12291" max="12291" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12547" max="12547" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12803" max="12803" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13059" max="13059" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13315" max="13315" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13571" max="13571" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13827" max="13827" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14083" max="14083" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14339" max="14339" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14595" max="14595" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14851" max="14851" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="15107" max="15107" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="15363" max="15363" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="15619" max="15619" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="15875" max="15875" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16131" max="16131" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="259" max="259" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="C7" s="8">
         <v>2019</v>
       </c>
@@ -4409,7 +4667,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="B8" s="9" t="s">
         <v>4</v>
       </c>
@@ -4423,7 +4681,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
@@ -4437,7 +4695,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" thickBot="1">
       <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
@@ -4451,7 +4709,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
@@ -4459,12 +4717,12 @@
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="B29" s="12" t="s">
         <v>8</v>
       </c>
@@ -4472,7 +4730,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="C31" s="8">
         <v>2019</v>
       </c>
@@ -4483,7 +4741,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="B32" s="9" t="s">
         <v>4</v>
       </c>
@@ -4497,7 +4755,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5">
       <c r="B33" s="9" t="s">
         <v>5</v>
       </c>
@@ -4511,7 +4769,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" ht="15" thickBot="1">
       <c r="B34" s="9" t="s">
         <v>6</v>
       </c>
@@ -4525,7 +4783,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5">
       <c r="B35" s="9" t="s">
         <v>9</v>
       </c>
@@ -4533,12 +4791,12 @@
       <c r="D35" s="44"/>
       <c r="E35" s="44"/>
     </row>
-    <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" ht="15" thickBot="1">
       <c r="B37" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5">
       <c r="B38" s="15"/>
       <c r="C38" s="16">
         <v>2019</v>
@@ -4550,7 +4808,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5">
       <c r="B39" s="18" t="s">
         <v>4</v>
       </c>
@@ -4564,7 +4822,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5">
       <c r="B40" s="18" t="s">
         <v>5</v>
       </c>
@@ -4578,7 +4836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" ht="15" thickBot="1">
       <c r="B41" s="18" t="s">
         <v>6</v>
       </c>
@@ -4592,7 +4850,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" ht="15" thickBot="1">
       <c r="B42" s="23" t="s">
         <v>9</v>
       </c>
@@ -4609,140 +4867,140 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>45</v>
       </c>
       <c r="E58" t="s">
         <v>47</v>
       </c>
-      <c r="F58" s="60">
+      <c r="F58" s="58">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="E59" t="s">
         <v>48</v>
       </c>
-      <c r="F59" s="60">
+      <c r="F59" s="58">
         <v>2</v>
       </c>
-      <c r="I59" s="66" t="s">
+      <c r="I59" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="J59" s="66"/>
-      <c r="K59" s="66"/>
-      <c r="L59" s="66"/>
-      <c r="M59" s="66"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B60" s="62" t="s">
+      <c r="J59" s="64"/>
+      <c r="K59" s="64"/>
+      <c r="L59" s="64"/>
+      <c r="M59" s="64"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="B60" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="C60" s="62" t="s">
+      <c r="C60" s="60" t="s">
         <v>46</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J60" s="69">
+      <c r="J60" s="67">
         <v>50</v>
       </c>
-      <c r="K60" s="69">
+      <c r="K60" s="67">
         <v>45</v>
       </c>
-      <c r="L60" s="69">
+      <c r="L60" s="67">
         <v>60</v>
       </c>
-      <c r="M60" s="70">
+      <c r="M60" s="68">
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="B61">
         <v>120</v>
       </c>
       <c r="C61">
         <v>50</v>
       </c>
-      <c r="E61" s="65" t="s">
+      <c r="E61" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="F61" s="64" t="s">
+      <c r="F61" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="I61" s="67">
+      <c r="I61" s="65">
         <v>120</v>
       </c>
-      <c r="J61" s="71"/>
-      <c r="K61" s="72"/>
-      <c r="L61" s="72"/>
-      <c r="M61" s="73"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J61" s="69"/>
+      <c r="K61" s="70"/>
+      <c r="L61" s="70"/>
+      <c r="M61" s="71"/>
+    </row>
+    <row r="62" spans="1:13">
       <c r="B62">
         <v>140</v>
       </c>
       <c r="C62">
         <v>45</v>
       </c>
-      <c r="I62" s="67">
+      <c r="I62" s="65">
         <v>140</v>
       </c>
-      <c r="J62" s="74"/>
-      <c r="K62" s="75"/>
-      <c r="L62" s="75"/>
-      <c r="M62" s="76"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J62" s="72"/>
+      <c r="K62" s="73"/>
+      <c r="L62" s="73"/>
+      <c r="M62" s="74"/>
+    </row>
+    <row r="63" spans="1:13">
       <c r="B63">
         <v>150</v>
       </c>
       <c r="C63">
         <v>60</v>
       </c>
-      <c r="I63" s="67">
+      <c r="I63" s="65">
         <v>150</v>
       </c>
-      <c r="J63" s="74"/>
-      <c r="K63" s="75"/>
-      <c r="L63" s="75"/>
-      <c r="M63" s="76"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J63" s="72"/>
+      <c r="K63" s="73"/>
+      <c r="L63" s="73"/>
+      <c r="M63" s="74"/>
+    </row>
+    <row r="64" spans="1:13">
       <c r="B64">
         <v>160</v>
       </c>
       <c r="C64">
         <v>70</v>
       </c>
-      <c r="I64" s="68">
+      <c r="I64" s="66">
         <v>160</v>
       </c>
-      <c r="J64" s="77"/>
-      <c r="K64" s="78"/>
-      <c r="L64" s="78"/>
-      <c r="M64" s="79"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J64" s="75"/>
+      <c r="K64" s="76"/>
+      <c r="L64" s="76"/>
+      <c r="M64" s="77"/>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="7" t="s">
         <v>53</v>
       </c>
       <c r="K70" s="26"/>
     </row>
-    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="15" thickBot="1"/>
+    <row r="72" spans="1:11" ht="15" thickBot="1">
       <c r="B72" s="27"/>
       <c r="C72" s="28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11">
       <c r="B73" s="29" t="s">
         <v>6</v>
       </c>
@@ -4750,7 +5008,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11">
       <c r="B74" s="29" t="s">
         <v>12</v>
       </c>
@@ -4758,7 +5016,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11">
       <c r="B75" s="29" t="s">
         <v>13</v>
       </c>
@@ -4766,7 +5024,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="15" thickBot="1">
       <c r="B76" s="32" t="s">
         <v>14</v>
       </c>
@@ -4774,54 +5032,72 @@
         <v>610</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11">
       <c r="B78" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="45"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C78" s="45">
+        <f>SUM(C73:C76)</f>
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="B79" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C79" s="46"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C79" s="46">
+        <f>AVERAGE(C73:C76)</f>
+        <v>554.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="B80" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C80" s="46"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="46">
+        <f>_xlfn.STDEV.S(C73:C76)</f>
+        <v>245.37114744810563</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="B81" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C81" s="45"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="45">
+        <f>MIN(C73:C76)</f>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="B82" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C82" s="45"/>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="45">
+        <f>MAX(C73:C76)</f>
+        <v>829</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15" thickBot="1"/>
+    <row r="84" spans="1:3" ht="15" thickBot="1">
       <c r="B84" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C84" s="47"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="47">
+        <f ca="1">TODAY()</f>
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="C91" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="B92" s="12" t="s">
         <v>1</v>
       </c>
@@ -4829,7 +5105,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="B93" s="12" t="s">
         <v>2</v>
       </c>
@@ -4837,7 +5113,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="B94" s="12" t="s">
         <v>3</v>
       </c>
@@ -4845,7 +5121,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="B95" s="12" t="s">
         <v>21</v>
       </c>
@@ -4853,47 +5129,56 @@
         <v>620</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="B97" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C97" s="34"/>
+      <c r="C97" s="34" t="str">
+        <f>IF(C92&gt;C93, "Q1 better than Q2", "Q2 better than Q1")</f>
+        <v>Q1 better than Q2</v>
+      </c>
       <c r="D97" s="35"/>
       <c r="E97" s="35"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="B99" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C99" s="34"/>
+      <c r="C99" s="34" t="str">
+        <f>IF(MAX(C92:C95)&gt;600, "Exc 600M in one quarter", "Quota not met")</f>
+        <v>Exc 600M in one quarter</v>
+      </c>
       <c r="D99" s="35"/>
       <c r="E99" s="35"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5">
       <c r="B101" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C101" s="34"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="66" t="s">
+    <row r="103" spans="1:5">
+      <c r="A103" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="C103" s="89"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="66" t="s">
+      <c r="C103" s="87" t="str">
+        <f>IF(OR(C92&lt;C94,C93&lt;C94), "Yes", "No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="C105" s="89"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="87"/>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="15" thickBot="1"/>
+    <row r="116" spans="1:3">
       <c r="B116" s="36" t="s">
         <v>8</v>
       </c>
@@ -4901,11 +5186,11 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="B117" s="38"/>
       <c r="C117" s="39"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="B118" s="38" t="s">
         <v>25</v>
       </c>
@@ -4913,7 +5198,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="15" thickBot="1">
       <c r="B119" s="38" t="s">
         <v>9</v>
       </c>
@@ -4922,7 +5207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="15" thickBot="1">
       <c r="B120" s="41" t="s">
         <v>7</v>
       </c>
@@ -4938,195 +5223,202 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="78" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="62">
+    <row r="2" spans="1:3">
+      <c r="A2" s="60">
         <v>2345</v>
       </c>
-      <c r="B2" s="62">
+      <c r="B2" s="60">
         <v>500</v>
       </c>
-      <c r="C2" s="93">
+      <c r="C2" s="89">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="62">
+    <row r="3" spans="1:3">
+      <c r="A3" s="60">
         <v>5457</v>
       </c>
-      <c r="B3" s="62">
+      <c r="B3" s="60">
         <v>234</v>
       </c>
-      <c r="C3" s="93">
+      <c r="C3" s="89">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="62">
+    <row r="4" spans="1:3">
+      <c r="A4" s="60">
         <v>9823</v>
       </c>
-      <c r="B4" s="62">
+      <c r="B4" s="60">
         <v>155</v>
       </c>
-      <c r="C4" s="93">
+      <c r="C4" s="89">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="62">
+    <row r="5" spans="1:3">
+      <c r="A5" s="60">
         <v>1233</v>
       </c>
-      <c r="B5" s="62">
+      <c r="B5" s="60">
         <v>122</v>
       </c>
-      <c r="C5" s="93">
+      <c r="C5" s="89">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="62">
+    <row r="6" spans="1:3">
+      <c r="A6" s="60">
         <v>2344</v>
       </c>
-      <c r="B6" s="62">
+      <c r="B6" s="60">
         <v>166</v>
       </c>
-      <c r="C6" s="93">
+      <c r="C6" s="89">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="62">
+    <row r="7" spans="1:3">
+      <c r="A7" s="60">
         <v>3363</v>
       </c>
-      <c r="B7" s="62">
+      <c r="B7" s="60">
         <v>145</v>
       </c>
-      <c r="C7" s="93">
+      <c r="C7" s="89">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="62">
+    <row r="8" spans="1:3">
+      <c r="A8" s="60">
         <v>5149</v>
       </c>
-      <c r="B8" s="62">
+      <c r="B8" s="60">
         <v>150</v>
       </c>
-      <c r="C8" s="93">
+      <c r="C8" s="89">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="62">
+    <row r="9" spans="1:3">
+      <c r="A9" s="60">
         <v>5329</v>
       </c>
-      <c r="B9" s="62">
+      <c r="B9" s="60">
         <v>320</v>
       </c>
-      <c r="C9" s="93">
+      <c r="C9" s="89">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="62">
+    <row r="10" spans="1:3">
+      <c r="A10" s="60">
         <v>6133</v>
       </c>
-      <c r="B10" s="62">
+      <c r="B10" s="60">
         <v>300</v>
       </c>
-      <c r="C10" s="93">
+      <c r="C10" s="89">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="62">
+    <row r="11" spans="1:3">
+      <c r="A11" s="60">
         <v>2700</v>
       </c>
-      <c r="B11" s="62">
+      <c r="B11" s="60">
         <v>80</v>
       </c>
-      <c r="C11" s="93">
+      <c r="C11" s="89">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="62">
+    <row r="12" spans="1:3">
+      <c r="A12" s="60">
         <v>5430</v>
       </c>
-      <c r="B12" s="62">
+      <c r="B12" s="60">
         <v>15</v>
       </c>
-      <c r="C12" s="93">
+      <c r="C12" s="89">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="62">
+    <row r="13" spans="1:3">
+      <c r="A13" s="60">
         <v>5088</v>
       </c>
-      <c r="B13" s="62">
+      <c r="B13" s="60">
         <v>410</v>
       </c>
-      <c r="C13" s="93">
+      <c r="C13" s="89">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="61">
+      <c r="B19" s="59">
         <v>6133</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64" t="s">
+      <c r="B21" s="61">
+        <f>VLOOKUP(6133,A2:C13,3,)</f>
+        <v>10</v>
+      </c>
+      <c r="C21" s="62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="B22">
+        <f>VLOOKUP(6133,A2:C13,2,)</f>
+        <v>300</v>
+      </c>
+      <c r="C22" s="62" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5136,160 +5428,262 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B70" sqref="B37:B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="62" t="s">
+      <c r="H4" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="62">
+      <c r="I4" s="60">
         <v>1958</v>
       </c>
-      <c r="J4" s="62">
+      <c r="J4" s="60">
         <v>1959</v>
       </c>
-      <c r="K4" s="62">
+      <c r="K4" s="60">
         <v>1960</v>
       </c>
       <c r="M4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+    <row r="5" spans="1:13">
+      <c r="A5" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="H5" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" s="59">
+        <v>340</v>
+      </c>
+      <c r="J5" s="59">
+        <v>360</v>
+      </c>
+      <c r="K5" s="59">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="81" t="s">
+      <c r="H6" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" s="59">
+        <v>318</v>
+      </c>
+      <c r="J6" s="59">
+        <v>342</v>
+      </c>
+      <c r="K6" s="59">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="81" t="s">
+      <c r="H7" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" s="59">
+        <v>362</v>
+      </c>
+      <c r="J7" s="59">
+        <v>406</v>
+      </c>
+      <c r="K7" s="59">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="81" t="s">
+      <c r="H8" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="I8" s="59">
+        <v>348</v>
+      </c>
+      <c r="J8" s="59">
+        <v>396</v>
+      </c>
+      <c r="K8" s="59">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
+      <c r="H9" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="I9" s="59">
+        <v>363</v>
+      </c>
+      <c r="J9" s="59">
+        <v>420</v>
+      </c>
+      <c r="K9" s="59">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="H10" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" s="59">
+        <v>435</v>
+      </c>
+      <c r="J10" s="59">
+        <v>472</v>
+      </c>
+      <c r="K10" s="59">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="81" t="s">
+      <c r="H11" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" s="59">
+        <v>491</v>
+      </c>
+      <c r="J11" s="59">
+        <v>548</v>
+      </c>
+      <c r="K11" s="59">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="81" t="s">
+      <c r="H12" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="I12" s="59">
+        <v>505</v>
+      </c>
+      <c r="J12" s="59">
+        <v>559</v>
+      </c>
+      <c r="K12" s="59">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="81" t="s">
+      <c r="H13" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="59">
+        <v>404</v>
+      </c>
+      <c r="J13" s="59">
+        <v>463</v>
+      </c>
+      <c r="K13" s="59">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="81" t="s">
+      <c r="H14" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="59">
+        <v>359</v>
+      </c>
+      <c r="J14" s="59">
+        <v>407</v>
+      </c>
+      <c r="K14" s="59">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="81" t="s">
+      <c r="H15" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="I15" s="59">
+        <v>310</v>
+      </c>
+      <c r="J15" s="59">
+        <v>362</v>
+      </c>
+      <c r="K15" s="59">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="81" t="s">
+      <c r="H16" s="59" t="s">
+        <v>153</v>
+      </c>
+      <c r="I16" s="59">
+        <v>337</v>
+      </c>
+      <c r="J16" s="59">
+        <v>405</v>
+      </c>
+      <c r="K16" s="59">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="G21" s="81" t="s">
+      <c r="G21" s="79" t="s">
         <v>88</v>
       </c>
       <c r="H21" t="s">
@@ -5308,449 +5702,719 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="81" t="s">
+    <row r="22" spans="1:13">
+      <c r="A22" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="81" t="s">
+      <c r="G22" s="59">
+        <v>1</v>
+      </c>
+      <c r="H22" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="I22" s="59">
+        <v>7.97</v>
+      </c>
+      <c r="J22" s="59">
+        <v>0.6</v>
+      </c>
+      <c r="K22" s="59">
+        <v>8.57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+      <c r="G23" s="59">
+        <v>2</v>
+      </c>
+      <c r="H23" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="I23" s="59">
+        <v>2.97</v>
+      </c>
+      <c r="J23" s="59">
+        <v>0.22</v>
+      </c>
+      <c r="K23" s="59">
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="81" t="s">
+      <c r="G24" s="59">
+        <v>3</v>
+      </c>
+      <c r="H24" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="I24" s="59">
+        <v>1.29</v>
+      </c>
+      <c r="J24" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="K24" s="59">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="81" t="s">
+      <c r="G25" s="59">
+        <v>4</v>
+      </c>
+      <c r="H25" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="I25" s="59">
+        <v>14.96</v>
+      </c>
+      <c r="J25" s="59">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="K25" s="59">
+        <v>16.079999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="81" t="s">
+      <c r="G26" s="59">
+        <v>5</v>
+      </c>
+      <c r="H26" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I26" s="59">
+        <v>7.28</v>
+      </c>
+      <c r="J26" s="59">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K26" s="59">
+        <v>7.83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="81" t="s">
+      <c r="G27" s="59">
+        <v>6</v>
+      </c>
+      <c r="H27" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="I27" s="59">
+        <v>6.68</v>
+      </c>
+      <c r="J27" s="59">
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="59">
+        <v>7.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="81" t="s">
+      <c r="G28" s="59">
+        <v>7</v>
+      </c>
+      <c r="H28" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="I28" s="59">
+        <v>10</v>
+      </c>
+      <c r="J28" s="59">
+        <v>0.75</v>
+      </c>
+      <c r="K28" s="59">
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="81" t="s">
+      <c r="G29" s="59">
+        <v>8</v>
+      </c>
+      <c r="H29" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29" s="59">
+        <v>8.98</v>
+      </c>
+      <c r="J29" s="59">
+        <v>0.67</v>
+      </c>
+      <c r="K29" s="59">
+        <v>9.65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="81" t="s">
+      <c r="G30" s="59">
+        <v>9</v>
+      </c>
+      <c r="H30" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I30" s="59">
+        <v>2.12</v>
+      </c>
+      <c r="J30" s="59">
+        <v>0.16</v>
+      </c>
+      <c r="K30" s="59">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="61"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="81"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" s="59">
+        <v>10</v>
+      </c>
+      <c r="H31" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="I31" s="59">
+        <v>6.19</v>
+      </c>
+      <c r="J31" s="59">
+        <v>0.46</v>
+      </c>
+      <c r="K31" s="59">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="79"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="59"/>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="83" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="84" t="s">
+      <c r="B35" s="82" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="64" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="82">
+    <row r="36" spans="1:5">
+      <c r="A36" s="80">
         <v>1</v>
       </c>
-      <c r="B36" s="85" t="s">
+      <c r="B36" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="61">
+      <c r="C36" s="59">
         <v>5379</v>
       </c>
       <c r="E36" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="82">
+    <row r="37" spans="1:5">
+      <c r="A37" s="80">
         <v>2</v>
       </c>
-      <c r="B37" s="82" t="s">
+      <c r="B37" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="61"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="82">
+      <c r="C37" s="59">
+        <v>5663</v>
+      </c>
+      <c r="D37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="80">
         <v>3</v>
       </c>
-      <c r="B38" s="82" t="s">
+      <c r="B38" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="61"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="82">
+      <c r="C38" s="59">
+        <v>5854</v>
+      </c>
+      <c r="D38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="80">
         <v>4</v>
       </c>
-      <c r="B39" s="82" t="s">
+      <c r="B39" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="61"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="82">
+      <c r="C39" s="59">
+        <v>6035</v>
+      </c>
+      <c r="D39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="80">
         <v>5</v>
       </c>
-      <c r="B40" s="82" t="s">
+      <c r="B40" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="61"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="82">
+      <c r="C40" s="59">
+        <v>6043</v>
+      </c>
+      <c r="D40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="80">
         <v>6</v>
       </c>
-      <c r="B41" s="82" t="s">
+      <c r="B41" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="61"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="82">
+      <c r="C41" s="59">
+        <v>6070</v>
+      </c>
+      <c r="D41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="80">
         <v>7</v>
       </c>
-      <c r="B42" s="82" t="s">
+      <c r="B42" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="61"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="82">
+      <c r="C42" s="59">
+        <v>6096</v>
+      </c>
+      <c r="D42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="80">
         <v>8</v>
       </c>
-      <c r="B43" s="82" t="s">
+      <c r="B43" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="C43" s="61"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="82">
+      <c r="C43" s="59">
+        <v>6119</v>
+      </c>
+      <c r="D43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="80">
         <v>9</v>
       </c>
-      <c r="B44" s="82" t="s">
+      <c r="B44" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="61"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="82">
+      <c r="C44" s="59">
+        <v>6136</v>
+      </c>
+      <c r="D44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="80">
         <v>10</v>
       </c>
-      <c r="B45" s="82" t="s">
+      <c r="B45" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="C45" s="61"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="82">
+      <c r="C45" s="59">
+        <v>6151</v>
+      </c>
+      <c r="D45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="80">
         <v>11</v>
       </c>
-      <c r="B46" s="82" t="s">
+      <c r="B46" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="61"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="82">
+      <c r="C46" s="59">
+        <v>6153</v>
+      </c>
+      <c r="D46" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="80">
         <v>12</v>
       </c>
-      <c r="B47" s="82" t="s">
+      <c r="B47" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="C47" s="61"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="82">
+      <c r="C47" s="59">
+        <v>6287</v>
+      </c>
+      <c r="D47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="80">
         <v>13</v>
       </c>
-      <c r="B48" s="82" t="s">
+      <c r="B48" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="61"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="82">
+      <c r="C48" s="59">
+        <v>6298</v>
+      </c>
+      <c r="D48" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="80">
         <v>14</v>
       </c>
-      <c r="B49" s="82" t="s">
+      <c r="B49" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="61"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="82">
+      <c r="C49" s="59">
+        <v>6313</v>
+      </c>
+      <c r="D49" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="80">
         <v>15</v>
       </c>
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="61"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="82">
+      <c r="C50" s="59">
+        <v>6327</v>
+      </c>
+      <c r="D50" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="80">
         <v>16</v>
       </c>
-      <c r="B51" s="82" t="s">
+      <c r="B51" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="C51" s="61"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="82">
+      <c r="C51" s="59">
+        <v>6333</v>
+      </c>
+      <c r="D51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="80">
         <v>17</v>
       </c>
-      <c r="B52" s="82" t="s">
+      <c r="B52" s="80" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="61"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="82">
+      <c r="C52" s="59">
+        <v>6389</v>
+      </c>
+      <c r="D52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="80">
         <v>18</v>
       </c>
-      <c r="B53" s="82" t="s">
+      <c r="B53" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="61"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="82">
+      <c r="C53" s="59">
+        <v>6413</v>
+      </c>
+      <c r="D53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="80">
         <v>19</v>
       </c>
-      <c r="B54" s="82" t="s">
+      <c r="B54" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="C54" s="61"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="82">
+      <c r="C54" s="59">
+        <v>6414</v>
+      </c>
+      <c r="D54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="80">
         <v>20</v>
       </c>
-      <c r="B55" s="82" t="s">
+      <c r="B55" s="80" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="61"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="82">
+      <c r="C55" s="59">
+        <v>6433</v>
+      </c>
+      <c r="D55" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="80">
         <v>21</v>
       </c>
-      <c r="B56" s="82" t="s">
+      <c r="B56" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="61"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="82">
+      <c r="C56" s="59">
+        <v>6499</v>
+      </c>
+      <c r="D56" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="80">
         <v>22</v>
       </c>
-      <c r="B57" s="82" t="s">
+      <c r="B57" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="61"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="82">
+      <c r="C57" s="59">
+        <v>6506</v>
+      </c>
+      <c r="D57" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="80">
         <v>23</v>
       </c>
-      <c r="B58" s="82" t="s">
+      <c r="B58" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="C58" s="61"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="82">
+      <c r="C58" s="59">
+        <v>6610</v>
+      </c>
+      <c r="D58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="80">
         <v>24</v>
       </c>
-      <c r="B59" s="82" t="s">
+      <c r="B59" s="80" t="s">
         <v>117</v>
       </c>
-      <c r="C59" s="61"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="82">
+      <c r="C59" s="59">
+        <v>6615</v>
+      </c>
+      <c r="D59" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="80">
         <v>25</v>
       </c>
-      <c r="B60" s="82" t="s">
+      <c r="B60" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="C60" s="61"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="82">
+      <c r="C60" s="59">
+        <v>6630</v>
+      </c>
+      <c r="D60" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="80">
         <v>26</v>
       </c>
-      <c r="B61" s="82" t="s">
+      <c r="B61" s="80" t="s">
         <v>119</v>
       </c>
-      <c r="C61" s="61"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="82">
+      <c r="C61" s="59">
+        <v>6636</v>
+      </c>
+      <c r="D61" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="80">
         <v>27</v>
       </c>
-      <c r="B62" s="82" t="s">
+      <c r="B62" s="80" t="s">
         <v>120</v>
       </c>
-      <c r="C62" s="61"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="82">
+      <c r="C62" s="59">
+        <v>6640</v>
+      </c>
+      <c r="D62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="80">
         <v>28</v>
       </c>
-      <c r="B63" s="82" t="s">
+      <c r="B63" s="80" t="s">
         <v>121</v>
       </c>
-      <c r="C63" s="61"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="82">
+      <c r="C63" s="59">
+        <v>6670</v>
+      </c>
+      <c r="D63" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="80">
         <v>29</v>
       </c>
-      <c r="B64" s="82" t="s">
+      <c r="B64" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C64" s="61"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="82">
+      <c r="C64" s="59">
+        <v>6691</v>
+      </c>
+      <c r="D64" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="80">
         <v>30</v>
       </c>
-      <c r="B65" s="82" t="s">
+      <c r="B65" s="80" t="s">
         <v>123</v>
       </c>
-      <c r="C65" s="61"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="82">
+      <c r="C65" s="59">
+        <v>6703</v>
+      </c>
+      <c r="D65" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="80">
         <v>31</v>
       </c>
-      <c r="B66" s="82" t="s">
+      <c r="B66" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="C66" s="61"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="82">
+      <c r="C66" s="59">
+        <v>6704</v>
+      </c>
+      <c r="D66" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="80">
         <v>32</v>
       </c>
-      <c r="B67" s="82" t="s">
+      <c r="B67" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="C67" s="61"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="82">
+      <c r="C67" s="59">
+        <v>6711</v>
+      </c>
+      <c r="D67" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="80">
         <v>33</v>
       </c>
-      <c r="B68" s="82" t="s">
+      <c r="B68" s="80" t="s">
         <v>126</v>
       </c>
-      <c r="C68" s="61"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="82">
+      <c r="C68" s="59">
+        <v>6712</v>
+      </c>
+      <c r="D68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="80">
         <v>34</v>
       </c>
-      <c r="B69" s="82" t="s">
+      <c r="B69" s="80" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="61"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="82">
+      <c r="C69" s="59">
+        <v>6714</v>
+      </c>
+      <c r="D69" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="80">
         <v>35</v>
       </c>
-      <c r="B70" s="82" t="s">
+      <c r="B70" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="C70" s="61"/>
+      <c r="C70" s="59">
+        <v>6728</v>
+      </c>
+      <c r="D70" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5758,22 +6422,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
         <v>135</v>
       </c>
@@ -5781,334 +6445,412 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="84" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="86" t="s">
         <v>42</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="50">
+    <row r="4" spans="1:7">
+      <c r="A4" s="49">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>9</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="50">
         <v>1957</v>
       </c>
-      <c r="F4" s="90"/>
-      <c r="G4" s="64" t="s">
+      <c r="F4" s="88" t="str">
+        <f>CONCATENATE(A4,"/",B4,"/",C4)</f>
+        <v>4/9/1957</v>
+      </c>
+      <c r="G4" s="62" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="52">
+    <row r="5" spans="1:7">
+      <c r="A5" s="51">
         <v>25</v>
       </c>
       <c r="B5" s="2">
         <v>7</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="52">
         <v>2000</v>
       </c>
-      <c r="F5" s="91"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="52">
+      <c r="F5" s="88" t="str">
+        <f t="shared" ref="F5:F29" si="0">CONCATENATE(A5,"/",B5,"/",C5)</f>
+        <v>25/7/2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="51">
         <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="53">
+      <c r="C6" s="52">
         <v>1966</v>
       </c>
-      <c r="F6" s="91"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
+      <c r="F6" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>8/4/1966</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="51">
         <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>8</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="52">
         <v>1972</v>
       </c>
-      <c r="F7" s="91"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="52">
+      <c r="F7" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>18/8/1972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="51">
         <v>26</v>
       </c>
       <c r="B8" s="2">
         <v>12</v>
       </c>
-      <c r="C8" s="53">
+      <c r="C8" s="52">
         <v>1992</v>
       </c>
-      <c r="F8" s="91"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="52">
+      <c r="F8" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>26/12/1992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="51">
         <v>26</v>
       </c>
       <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="53">
+      <c r="C9" s="52">
         <v>1978</v>
       </c>
-      <c r="F9" s="91"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="52">
+      <c r="F9" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>26/6/1978</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="51">
         <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>4</v>
       </c>
-      <c r="C10" s="53">
+      <c r="C10" s="52">
         <v>1999</v>
       </c>
-      <c r="F10" s="91"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="52">
+      <c r="F10" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>14/4/1999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="51">
         <v>19</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="53">
+      <c r="C11" s="52">
         <v>1990</v>
       </c>
-      <c r="F11" s="91"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="52">
+      <c r="F11" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>19/10/1990</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="51">
         <v>4</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="52">
         <v>1965</v>
       </c>
-      <c r="F12" s="91"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="52">
+      <c r="F12" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>4/2/1965</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="51">
         <v>14</v>
       </c>
       <c r="B13" s="2">
         <v>7</v>
       </c>
-      <c r="C13" s="53">
+      <c r="C13" s="52">
         <v>1969</v>
       </c>
-      <c r="F13" s="91"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="52">
+      <c r="F13" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>14/7/1969</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="51">
         <v>6</v>
       </c>
       <c r="B14" s="2">
         <v>7</v>
       </c>
-      <c r="C14" s="53">
+      <c r="C14" s="52">
         <v>1995</v>
       </c>
-      <c r="F14" s="91"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="52">
+      <c r="F14" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>6/7/1995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="51">
         <v>8</v>
       </c>
       <c r="B15" s="2">
         <v>10</v>
       </c>
-      <c r="C15" s="53">
+      <c r="C15" s="52">
         <v>1996</v>
       </c>
-      <c r="F15" s="91"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="52">
+      <c r="F15" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>8/10/1996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="51">
         <v>29</v>
       </c>
       <c r="B16" s="2">
         <v>8</v>
       </c>
-      <c r="C16" s="53">
+      <c r="C16" s="52">
         <v>1975</v>
       </c>
-      <c r="F16" s="91"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="52">
+      <c r="F16" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>29/8/1975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="51">
         <v>22</v>
       </c>
       <c r="B17" s="2">
         <v>11</v>
       </c>
-      <c r="C17" s="53">
+      <c r="C17" s="52">
         <v>1994</v>
       </c>
-      <c r="F17" s="91"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="52">
+      <c r="F17" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>22/11/1994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="51">
         <v>28</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="53">
+      <c r="C18" s="52">
         <v>1965</v>
       </c>
-      <c r="F18" s="91"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
+      <c r="F18" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>28/1/1965</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="51">
         <v>4</v>
       </c>
       <c r="B19" s="2">
         <v>9</v>
       </c>
-      <c r="C19" s="53">
+      <c r="C19" s="52">
         <v>1989</v>
       </c>
-      <c r="F19" s="91"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="52">
+      <c r="F19" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>4/9/1989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="51">
         <v>2</v>
       </c>
       <c r="B20" s="2">
         <v>10</v>
       </c>
-      <c r="C20" s="53">
+      <c r="C20" s="52">
         <v>1984</v>
       </c>
-      <c r="F20" s="91"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="52">
+      <c r="F20" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>2/10/1984</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="51">
         <v>22</v>
       </c>
       <c r="B21" s="2">
         <v>3</v>
       </c>
-      <c r="C21" s="53">
+      <c r="C21" s="52">
         <v>2000</v>
       </c>
-      <c r="F21" s="91"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="52">
+      <c r="F21" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>22/3/2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="51">
         <v>7</v>
       </c>
       <c r="B22" s="2">
         <v>8</v>
       </c>
-      <c r="C22" s="53">
+      <c r="C22" s="52">
         <v>1966</v>
       </c>
-      <c r="F22" s="91"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="52">
+      <c r="F22" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>7/8/1966</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="51">
         <v>25</v>
       </c>
       <c r="B23" s="2">
         <v>3</v>
       </c>
-      <c r="C23" s="53">
+      <c r="C23" s="52">
         <v>1987</v>
       </c>
-      <c r="F23" s="91"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="52">
+      <c r="F23" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>25/3/1987</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="51">
         <v>3</v>
       </c>
       <c r="B24" s="2">
         <v>10</v>
       </c>
-      <c r="C24" s="53">
+      <c r="C24" s="52">
         <v>1994</v>
       </c>
-      <c r="F24" s="91"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="52">
+      <c r="F24" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>3/10/1994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="51">
         <v>25</v>
       </c>
       <c r="B25" s="2">
         <v>7</v>
       </c>
-      <c r="C25" s="53">
+      <c r="C25" s="52">
         <v>1976</v>
       </c>
-      <c r="F25" s="91"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="52">
+      <c r="F25" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>25/7/1976</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="51">
         <v>26</v>
       </c>
       <c r="B26" s="2">
         <v>2</v>
       </c>
-      <c r="C26" s="53">
+      <c r="C26" s="52">
         <v>1999</v>
       </c>
-      <c r="F26" s="91"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="52">
+      <c r="F26" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>26/2/1999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="51">
         <v>8</v>
       </c>
       <c r="B27" s="2">
         <v>12</v>
       </c>
-      <c r="C27" s="53">
+      <c r="C27" s="52">
         <v>1980</v>
       </c>
-      <c r="F27" s="91"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="52">
+      <c r="F27" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>8/12/1980</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="51">
         <v>6</v>
       </c>
       <c r="B28" s="2">
         <v>8</v>
       </c>
-      <c r="C28" s="53">
+      <c r="C28" s="52">
         <v>1974</v>
       </c>
-      <c r="F28" s="91"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="55">
+      <c r="F28" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>6/8/1974</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="54">
         <v>24</v>
       </c>
       <c r="B29" s="3">
         <v>7</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="55">
         <v>1973</v>
       </c>
-      <c r="F29" s="92"/>
+      <c r="F29" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>24/7/1973</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>